<commit_message>
save results and other stuff
</commit_message>
<xml_diff>
--- a/results_BRS.xlsx
+++ b/results_BRS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374A504C-6231-4124-B542-80993AE4FB34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAFCEBB-EDF9-4FE2-9EE7-2B060A59B276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AD40" sqref="AD40"/>
     </sheetView>
   </sheetViews>
@@ -3059,20 +3059,12 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="Z24:AC24"/>
+    <mergeCell ref="Z28:AC28"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="Z23:AC23"/>
     <mergeCell ref="U3:X3"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U8:X8"/>
@@ -3089,12 +3081,20 @@
     <mergeCell ref="K4:N4"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="P3:S3"/>
-    <mergeCell ref="Z24:AC24"/>
-    <mergeCell ref="Z28:AC28"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="Z3:AC3"/>
-    <mergeCell ref="Z8:AC8"/>
-    <mergeCell ref="Z23:AC23"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="F8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
modified structure and README
</commit_message>
<xml_diff>
--- a/results_BRS.xlsx
+++ b/results_BRS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAFCEBB-EDF9-4FE2-9EE7-2B060A59B276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6593EDA8-F5B0-4805-9A8F-A0D052EDC94E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ISIP 2020 Overview" sheetId="1" r:id="rId1"/>
@@ -629,7 +629,7 @@
   <dimension ref="A1:AC41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD40" sqref="AD40"/>
+      <selection activeCell="AJ30" sqref="AJ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,13 +1070,13 @@
         <v>2</v>
       </c>
       <c r="L11" s="3">
-        <v>-1</v>
+        <v>364</v>
       </c>
       <c r="M11" s="3">
-        <v>-1</v>
+        <v>358</v>
       </c>
       <c r="N11" s="2">
-        <v>-1</v>
+        <v>461.55</v>
       </c>
       <c r="P11" s="9">
         <v>2</v>
@@ -1094,13 +1094,13 @@
         <v>2</v>
       </c>
       <c r="V11" s="3">
-        <v>-1</v>
+        <v>380</v>
       </c>
       <c r="W11" s="3">
-        <v>-1</v>
+        <v>387</v>
       </c>
       <c r="X11" s="2">
-        <v>-1</v>
+        <v>504.86</v>
       </c>
       <c r="Z11" s="9">
         <v>2</v>
@@ -1144,13 +1144,13 @@
         <v>3</v>
       </c>
       <c r="L12" s="3">
-        <v>-1</v>
+        <v>414</v>
       </c>
       <c r="M12" s="3">
-        <v>-1</v>
+        <v>427</v>
       </c>
       <c r="N12" s="2">
-        <v>-1</v>
+        <v>421.18</v>
       </c>
       <c r="P12" s="9">
         <v>3</v>
@@ -1168,25 +1168,25 @@
         <v>3</v>
       </c>
       <c r="V12" s="3">
-        <v>-1</v>
+        <v>434</v>
       </c>
       <c r="W12" s="3">
-        <v>-1</v>
+        <v>445</v>
       </c>
       <c r="X12" s="2">
-        <v>-1</v>
+        <v>442.04</v>
       </c>
       <c r="Z12" s="9">
         <v>3</v>
       </c>
       <c r="AA12" s="3">
-        <v>-1</v>
+        <v>500</v>
       </c>
       <c r="AB12" s="3">
-        <v>-1</v>
+        <v>366</v>
       </c>
       <c r="AC12" s="2">
-        <v>-1</v>
+        <v>424.18</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
@@ -1194,13 +1194,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="3">
-        <v>886</v>
+        <v>811</v>
       </c>
       <c r="C13" s="3">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D13" s="2">
-        <v>503.4</v>
+        <v>502.02</v>
       </c>
       <c r="F13" s="9">
         <v>4</v>
@@ -1218,49 +1218,49 @@
         <v>4</v>
       </c>
       <c r="L13" s="3">
-        <v>-1</v>
+        <v>504</v>
       </c>
       <c r="M13" s="3">
-        <v>-1</v>
+        <v>424</v>
       </c>
       <c r="N13" s="2">
-        <v>-1</v>
+        <v>373.57</v>
       </c>
       <c r="P13" s="9">
         <v>4</v>
       </c>
       <c r="Q13" s="3">
-        <v>-1</v>
+        <v>459</v>
       </c>
       <c r="R13" s="3">
-        <v>-1</v>
+        <v>421</v>
       </c>
       <c r="S13" s="2">
-        <v>-1</v>
+        <v>364.21</v>
       </c>
       <c r="U13" s="9">
         <v>4</v>
       </c>
       <c r="V13" s="3">
-        <v>-1</v>
+        <v>515</v>
       </c>
       <c r="W13" s="3">
-        <v>-1</v>
+        <v>426</v>
       </c>
       <c r="X13" s="2">
-        <v>-1</v>
+        <v>364.49</v>
       </c>
       <c r="Z13" s="9">
         <v>4</v>
       </c>
       <c r="AA13" s="3">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="AB13" s="3">
-        <v>228</v>
+        <v>410</v>
       </c>
       <c r="AC13" s="2">
-        <v>601.85</v>
+        <v>356.82</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -1268,73 +1268,73 @@
         <v>5</v>
       </c>
       <c r="B14" s="3">
-        <v>747</v>
+        <v>735</v>
       </c>
       <c r="C14" s="3">
-        <v>536</v>
+        <v>483</v>
       </c>
       <c r="D14" s="2">
-        <v>430.37</v>
+        <v>430.01</v>
       </c>
       <c r="F14" s="9">
         <v>5</v>
       </c>
       <c r="G14" s="3">
-        <v>302</v>
+        <v>-1</v>
       </c>
       <c r="H14" s="3">
-        <v>428</v>
+        <v>-1</v>
       </c>
       <c r="I14" s="2">
-        <v>494.94</v>
+        <v>-1</v>
       </c>
       <c r="K14" s="9">
         <v>5</v>
       </c>
       <c r="L14" s="3">
-        <v>-1</v>
+        <v>557</v>
       </c>
       <c r="M14" s="3">
-        <v>-1</v>
+        <v>358</v>
       </c>
       <c r="N14" s="2">
-        <v>-1</v>
+        <v>315.02</v>
       </c>
       <c r="P14" s="9">
         <v>5</v>
       </c>
       <c r="Q14" s="3">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="R14" s="3">
-        <v>421</v>
+        <v>316</v>
       </c>
       <c r="S14" s="2">
-        <v>364.21</v>
+        <v>287.27999999999997</v>
       </c>
       <c r="U14" s="9">
         <v>5</v>
       </c>
       <c r="V14" s="3">
-        <v>-1</v>
+        <v>534</v>
       </c>
       <c r="W14" s="3">
-        <v>-1</v>
+        <v>346</v>
       </c>
       <c r="X14" s="2">
-        <v>-1</v>
+        <v>297.45999999999998</v>
       </c>
       <c r="Z14" s="9">
         <v>5</v>
       </c>
       <c r="AA14" s="3">
-        <v>604</v>
+        <v>682</v>
       </c>
       <c r="AB14" s="3">
-        <v>410</v>
+        <v>347</v>
       </c>
       <c r="AC14" s="2">
-        <v>356.82</v>
+        <v>311.2</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
@@ -1342,73 +1342,73 @@
         <v>6</v>
       </c>
       <c r="B15" s="3">
-        <v>628</v>
+        <v>643</v>
       </c>
       <c r="C15" s="3">
-        <v>526</v>
+        <v>454</v>
       </c>
       <c r="D15" s="2">
-        <v>382.19</v>
+        <v>362.89</v>
       </c>
       <c r="F15" s="9">
         <v>6</v>
       </c>
       <c r="G15" s="3">
-        <v>382</v>
+        <v>-1</v>
       </c>
       <c r="H15" s="3">
-        <v>487</v>
+        <v>-1</v>
       </c>
       <c r="I15" s="2">
-        <v>425.18</v>
+        <v>-1</v>
       </c>
       <c r="K15" s="9">
         <v>6</v>
       </c>
       <c r="L15" s="3">
-        <v>-1</v>
+        <v>527</v>
       </c>
       <c r="M15" s="3">
-        <v>-1</v>
+        <v>279</v>
       </c>
       <c r="N15" s="2">
-        <v>-1</v>
+        <v>241.5</v>
       </c>
       <c r="P15" s="9">
         <v>6</v>
       </c>
       <c r="Q15" s="3">
-        <v>453</v>
+        <v>359</v>
       </c>
       <c r="R15" s="3">
-        <v>316</v>
+        <v>252</v>
       </c>
       <c r="S15" s="2">
-        <v>287.27999999999997</v>
+        <v>219.81</v>
       </c>
       <c r="U15" s="9">
         <v>6</v>
       </c>
       <c r="V15" s="3">
-        <v>-1</v>
+        <v>478</v>
       </c>
       <c r="W15" s="3">
-        <v>-1</v>
+        <v>280</v>
       </c>
       <c r="X15" s="2">
-        <v>-1</v>
+        <v>244.37</v>
       </c>
       <c r="Z15" s="9">
         <v>6</v>
       </c>
       <c r="AA15" s="3">
-        <v>682</v>
+        <v>666</v>
       </c>
       <c r="AB15" s="3">
-        <v>347</v>
+        <v>240</v>
       </c>
       <c r="AC15" s="2">
-        <v>311.2</v>
+        <v>263.97000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -1428,13 +1428,13 @@
         <v>7</v>
       </c>
       <c r="G16" s="3">
-        <v>503</v>
+        <v>392</v>
       </c>
       <c r="H16" s="3">
-        <v>458</v>
+        <v>270</v>
       </c>
       <c r="I16" s="2">
-        <v>344.92</v>
+        <v>230.28</v>
       </c>
       <c r="K16" s="9">
         <v>7</v>
@@ -1452,37 +1452,37 @@
         <v>7</v>
       </c>
       <c r="Q16" s="3">
-        <v>359</v>
+        <v>250</v>
       </c>
       <c r="R16" s="3">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="S16" s="2">
-        <v>219.81</v>
+        <v>179.59</v>
       </c>
       <c r="U16" s="9">
         <v>7</v>
       </c>
       <c r="V16" s="3">
-        <v>-1</v>
+        <v>397</v>
       </c>
       <c r="W16" s="3">
-        <v>-1</v>
+        <v>258</v>
       </c>
       <c r="X16" s="2">
-        <v>-1</v>
+        <v>208.78</v>
       </c>
       <c r="Z16" s="9">
         <v>7</v>
       </c>
       <c r="AA16" s="3">
-        <v>666</v>
+        <v>576</v>
       </c>
       <c r="AB16" s="3">
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="AC16" s="2">
-        <v>263.97000000000003</v>
+        <v>215.04</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
@@ -1502,13 +1502,13 @@
         <v>8</v>
       </c>
       <c r="G17" s="3">
-        <v>392</v>
+        <v>272</v>
       </c>
       <c r="H17" s="3">
-        <v>270</v>
+        <v>344</v>
       </c>
       <c r="I17" s="2">
-        <v>230.28</v>
+        <v>172.05</v>
       </c>
       <c r="K17" s="9">
         <v>8</v>
@@ -1526,37 +1526,37 @@
         <v>8</v>
       </c>
       <c r="Q17" s="3">
-        <v>250</v>
+        <v>185</v>
       </c>
       <c r="R17" s="3">
-        <v>269</v>
+        <v>349</v>
       </c>
       <c r="S17" s="2">
-        <v>179.59</v>
+        <v>149.61000000000001</v>
       </c>
       <c r="U17" s="9">
         <v>8</v>
       </c>
       <c r="V17" s="3">
-        <v>-1</v>
+        <v>324</v>
       </c>
       <c r="W17" s="3">
-        <v>-1</v>
+        <v>318</v>
       </c>
       <c r="X17" s="2">
-        <v>-1</v>
+        <v>171.97</v>
       </c>
       <c r="Z17" s="9">
         <v>8</v>
       </c>
       <c r="AA17" s="3">
-        <v>576</v>
+        <v>474</v>
       </c>
       <c r="AB17" s="3">
-        <v>180</v>
+        <v>229</v>
       </c>
       <c r="AC17" s="2">
-        <v>215.04</v>
+        <v>158.82</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
@@ -1564,25 +1564,25 @@
         <v>9</v>
       </c>
       <c r="B18" s="3">
-        <v>767</v>
+        <v>857</v>
       </c>
       <c r="C18" s="3">
-        <v>256</v>
+        <v>315</v>
       </c>
       <c r="D18" s="2">
-        <v>219.61</v>
+        <v>180.2</v>
       </c>
       <c r="F18" s="9">
         <v>9</v>
       </c>
       <c r="G18" s="3">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H18" s="3">
-        <v>344</v>
+        <v>481</v>
       </c>
       <c r="I18" s="2">
-        <v>172.05</v>
+        <v>115.37</v>
       </c>
       <c r="K18" s="9">
         <v>9</v>
@@ -1600,25 +1600,25 @@
         <v>9</v>
       </c>
       <c r="Q18" s="3">
-        <v>185</v>
+        <v>213</v>
       </c>
       <c r="R18" s="3">
-        <v>349</v>
+        <v>458</v>
       </c>
       <c r="S18" s="2">
-        <v>149.61000000000001</v>
+        <v>117.43</v>
       </c>
       <c r="U18" s="9">
         <v>9</v>
       </c>
       <c r="V18" s="3">
-        <v>534</v>
+        <v>308</v>
       </c>
       <c r="W18" s="3">
-        <v>346</v>
+        <v>402</v>
       </c>
       <c r="X18" s="2">
-        <v>297.45999999999998</v>
+        <v>139.97999999999999</v>
       </c>
       <c r="Z18" s="9">
         <v>9</v>
@@ -1638,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="B19" s="3">
-        <v>857</v>
+        <v>831</v>
       </c>
       <c r="C19" s="3">
-        <v>315</v>
+        <v>507</v>
       </c>
       <c r="D19" s="2">
-        <v>180.2</v>
+        <v>105.26</v>
       </c>
       <c r="F19" s="9">
         <v>10</v>
@@ -1674,25 +1674,25 @@
         <v>10</v>
       </c>
       <c r="Q19" s="3">
-        <v>213</v>
+        <v>294</v>
       </c>
       <c r="R19" s="3">
-        <v>458</v>
+        <v>508</v>
       </c>
       <c r="S19" s="2">
-        <v>117.43</v>
+        <v>89.02</v>
       </c>
       <c r="U19" s="9">
         <v>10</v>
       </c>
       <c r="V19" s="3">
-        <v>478</v>
+        <v>344</v>
       </c>
       <c r="W19" s="3">
-        <v>280</v>
+        <v>464</v>
       </c>
       <c r="X19" s="2">
-        <v>244.37</v>
+        <v>112.66</v>
       </c>
       <c r="Z19" s="9">
         <v>10</v>
@@ -1712,13 +1712,13 @@
         <v>11</v>
       </c>
       <c r="B20" s="3">
-        <v>831</v>
+        <v>628</v>
       </c>
       <c r="C20" s="3">
-        <v>507</v>
+        <v>526</v>
       </c>
       <c r="D20" s="2">
-        <v>105.26</v>
+        <v>22.19</v>
       </c>
       <c r="F20" s="9">
         <v>11</v>
@@ -1760,13 +1760,13 @@
         <v>11</v>
       </c>
       <c r="V20" s="3">
-        <v>397</v>
+        <v>508</v>
       </c>
       <c r="W20" s="3">
-        <v>258</v>
+        <v>516</v>
       </c>
       <c r="X20" s="2">
-        <v>208.78</v>
+        <v>37.28</v>
       </c>
       <c r="Z20" s="9">
         <v>11</v>
@@ -2210,13 +2210,13 @@
         <v>1</v>
       </c>
       <c r="Q30" s="3">
-        <v>-1</v>
+        <v>362</v>
       </c>
       <c r="R30" s="3">
-        <v>-1</v>
+        <v>317</v>
       </c>
       <c r="S30" s="2">
-        <v>-1</v>
+        <v>545.41</v>
       </c>
       <c r="U30" s="9">
         <v>1</v>
@@ -2284,13 +2284,13 @@
         <v>2</v>
       </c>
       <c r="Q31" s="3">
-        <v>-1</v>
+        <v>359</v>
       </c>
       <c r="R31" s="3">
-        <v>-1</v>
+        <v>408</v>
       </c>
       <c r="S31" s="2">
-        <v>-1</v>
+        <v>479.97</v>
       </c>
       <c r="U31" s="9">
         <v>2</v>
@@ -2308,13 +2308,13 @@
         <v>2</v>
       </c>
       <c r="AA31" s="3">
-        <v>-1</v>
+        <v>360</v>
       </c>
       <c r="AB31" s="3">
-        <v>-1</v>
+        <v>334</v>
       </c>
       <c r="AC31" s="2">
-        <v>-1</v>
+        <v>563.13</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
@@ -2358,13 +2358,13 @@
         <v>3</v>
       </c>
       <c r="Q32" s="3">
-        <v>-1</v>
+        <v>446</v>
       </c>
       <c r="R32" s="3">
-        <v>-1</v>
+        <v>440</v>
       </c>
       <c r="S32" s="2">
-        <v>-1</v>
+        <v>406.48</v>
       </c>
       <c r="U32" s="9">
         <v>3</v>
@@ -2420,37 +2420,37 @@
         <v>4</v>
       </c>
       <c r="L33" s="3">
-        <v>-1</v>
+        <v>570</v>
       </c>
       <c r="M33" s="3">
-        <v>-1</v>
+        <v>432</v>
       </c>
       <c r="N33" s="2">
-        <v>-1</v>
+        <v>364.98</v>
       </c>
       <c r="P33" s="9">
         <v>4</v>
       </c>
       <c r="Q33" s="3">
-        <v>-1</v>
+        <v>520</v>
       </c>
       <c r="R33" s="3">
-        <v>-1</v>
+        <v>382</v>
       </c>
       <c r="S33" s="2">
-        <v>-1</v>
+        <v>336.72</v>
       </c>
       <c r="U33" s="9">
         <v>4</v>
       </c>
       <c r="V33" s="3">
-        <v>343</v>
+        <v>409</v>
       </c>
       <c r="W33" s="3">
-        <v>284</v>
+        <v>394</v>
       </c>
       <c r="X33" s="2">
-        <v>513.04</v>
+        <v>465.2</v>
       </c>
       <c r="Z33" s="9">
         <v>4</v>
@@ -2494,37 +2494,37 @@
         <v>5</v>
       </c>
       <c r="L34" s="3">
-        <v>570</v>
+        <v>612</v>
       </c>
       <c r="M34" s="3">
-        <v>432</v>
+        <v>322</v>
       </c>
       <c r="N34" s="2">
-        <v>364.98</v>
+        <v>301.68</v>
       </c>
       <c r="P34" s="9">
         <v>5</v>
       </c>
       <c r="Q34" s="3">
-        <v>-1</v>
+        <v>519</v>
       </c>
       <c r="R34" s="3">
-        <v>-1</v>
+        <v>292</v>
       </c>
       <c r="S34" s="2">
-        <v>-1</v>
+        <v>287.22000000000003</v>
       </c>
       <c r="U34" s="9">
         <v>5</v>
       </c>
       <c r="V34" s="3">
-        <v>375</v>
+        <v>512</v>
       </c>
       <c r="W34" s="3">
-        <v>494</v>
+        <v>460</v>
       </c>
       <c r="X34" s="2">
-        <v>436.23</v>
+        <v>381.46</v>
       </c>
       <c r="Z34" s="9">
         <v>5</v>
@@ -2544,49 +2544,49 @@
         <v>6</v>
       </c>
       <c r="B35" s="3">
-        <v>-1</v>
+        <v>546</v>
       </c>
       <c r="C35" s="3">
-        <v>-1</v>
+        <v>216</v>
       </c>
       <c r="D35" s="2">
-        <v>-1</v>
+        <v>251.18</v>
       </c>
       <c r="F35" s="9">
         <v>6</v>
       </c>
       <c r="G35" s="3">
-        <v>-1</v>
+        <v>542</v>
       </c>
       <c r="H35" s="3">
-        <v>-1</v>
+        <v>240</v>
       </c>
       <c r="I35" s="2">
-        <v>-1</v>
+        <v>261.01</v>
       </c>
       <c r="K35" s="9">
         <v>6</v>
       </c>
       <c r="L35" s="3">
-        <v>612</v>
+        <v>534</v>
       </c>
       <c r="M35" s="3">
-        <v>322</v>
+        <v>236</v>
       </c>
       <c r="N35" s="2">
-        <v>301.68</v>
+        <v>251.13</v>
       </c>
       <c r="P35" s="9">
         <v>6</v>
       </c>
       <c r="Q35" s="3">
-        <v>362</v>
+        <v>449</v>
       </c>
       <c r="R35" s="3">
-        <v>317</v>
+        <v>236</v>
       </c>
       <c r="S35" s="2">
-        <v>545.41</v>
+        <v>246.12</v>
       </c>
       <c r="U35" s="9">
         <v>6</v>
@@ -2618,49 +2618,49 @@
         <v>7</v>
       </c>
       <c r="B36" s="3">
-        <v>546</v>
+        <v>450</v>
       </c>
       <c r="C36" s="3">
-        <v>216</v>
+        <v>171</v>
       </c>
       <c r="D36" s="2">
-        <v>251.18</v>
+        <v>209.57</v>
       </c>
       <c r="F36" s="9">
         <v>7</v>
       </c>
       <c r="G36" s="3">
-        <v>-1</v>
+        <v>448</v>
       </c>
       <c r="H36" s="3">
-        <v>-1</v>
+        <v>179</v>
       </c>
       <c r="I36" s="2">
-        <v>-1</v>
+        <v>220.79</v>
       </c>
       <c r="K36" s="9">
         <v>7</v>
       </c>
       <c r="L36" s="3">
-        <v>534</v>
+        <v>414</v>
       </c>
       <c r="M36" s="3">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="N36" s="2">
-        <v>251.13</v>
+        <v>206.87</v>
       </c>
       <c r="P36" s="9">
         <v>7</v>
       </c>
       <c r="Q36" s="3">
-        <v>520</v>
+        <v>344</v>
       </c>
       <c r="R36" s="3">
-        <v>382</v>
+        <v>258</v>
       </c>
       <c r="S36" s="2">
-        <v>336.72</v>
+        <v>200.32</v>
       </c>
       <c r="U36" s="9">
         <v>7</v>
@@ -2692,49 +2692,49 @@
         <v>8</v>
       </c>
       <c r="B37" s="3">
-        <v>450</v>
+        <v>357</v>
       </c>
       <c r="C37" s="3">
-        <v>171</v>
+        <v>209</v>
       </c>
       <c r="D37" s="2">
-        <v>209.57</v>
+        <v>175.5</v>
       </c>
       <c r="F37" s="9">
         <v>8</v>
       </c>
       <c r="G37" s="3">
-        <v>-1</v>
+        <v>335</v>
       </c>
       <c r="H37" s="3">
-        <v>-1</v>
+        <v>202</v>
       </c>
       <c r="I37" s="2">
-        <v>-1</v>
+        <v>186.02</v>
       </c>
       <c r="K37" s="9">
         <v>8</v>
       </c>
       <c r="L37" s="3">
-        <v>414</v>
+        <v>325</v>
       </c>
       <c r="M37" s="3">
-        <v>228</v>
+        <v>306</v>
       </c>
       <c r="N37" s="2">
-        <v>206.87</v>
+        <v>168.35</v>
       </c>
       <c r="P37" s="9">
         <v>8</v>
       </c>
       <c r="Q37" s="3">
-        <v>519</v>
+        <v>290</v>
       </c>
       <c r="R37" s="3">
-        <v>292</v>
+        <v>327</v>
       </c>
       <c r="S37" s="2">
-        <v>287.22000000000003</v>
+        <v>165</v>
       </c>
       <c r="U37" s="9">
         <v>8</v>
@@ -2766,49 +2766,49 @@
         <v>9</v>
       </c>
       <c r="B38" s="3">
-        <v>357</v>
+        <v>319</v>
       </c>
       <c r="C38" s="3">
-        <v>209</v>
+        <v>312</v>
       </c>
       <c r="D38" s="2">
-        <v>175.5</v>
+        <v>139.13</v>
       </c>
       <c r="F38" s="9">
         <v>9</v>
       </c>
       <c r="G38" s="3">
-        <v>542</v>
+        <v>266</v>
       </c>
       <c r="H38" s="3">
-        <v>240</v>
+        <v>302</v>
       </c>
       <c r="I38" s="2">
-        <v>261.01</v>
+        <v>151.85</v>
       </c>
       <c r="K38" s="9">
         <v>9</v>
       </c>
       <c r="L38" s="3">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="M38" s="3">
-        <v>306</v>
+        <v>426</v>
       </c>
       <c r="N38" s="2">
-        <v>168.35</v>
+        <v>131.35</v>
       </c>
       <c r="P38" s="9">
         <v>9</v>
       </c>
       <c r="Q38" s="3">
-        <v>449</v>
+        <v>319</v>
       </c>
       <c r="R38" s="3">
-        <v>236</v>
+        <v>434</v>
       </c>
       <c r="S38" s="2">
-        <v>246.12</v>
+        <v>118.28</v>
       </c>
       <c r="U38" s="9">
         <v>9</v>
@@ -2840,49 +2840,49 @@
         <v>10</v>
       </c>
       <c r="B39" s="3">
-        <v>319</v>
+        <v>348</v>
       </c>
       <c r="C39" s="3">
-        <v>312</v>
+        <v>414</v>
       </c>
       <c r="D39" s="2">
-        <v>139.13</v>
+        <v>103.11</v>
       </c>
       <c r="F39" s="9">
         <v>10</v>
       </c>
       <c r="G39" s="3">
-        <v>448</v>
+        <v>270</v>
       </c>
       <c r="H39" s="3">
-        <v>179</v>
+        <v>426</v>
       </c>
       <c r="I39" s="2">
-        <v>220.79</v>
+        <v>117.95</v>
       </c>
       <c r="K39" s="9">
         <v>10</v>
       </c>
       <c r="L39" s="3">
-        <v>311</v>
+        <v>379</v>
       </c>
       <c r="M39" s="3">
-        <v>426</v>
+        <v>500</v>
       </c>
       <c r="N39" s="2">
-        <v>131.35</v>
+        <v>100.2</v>
       </c>
       <c r="P39" s="9">
         <v>10</v>
       </c>
       <c r="Q39" s="3">
-        <v>344</v>
+        <v>436</v>
       </c>
       <c r="R39" s="3">
-        <v>258</v>
+        <v>506</v>
       </c>
       <c r="S39" s="2">
-        <v>200.32</v>
+        <v>56.32</v>
       </c>
       <c r="U39" s="9">
         <v>10</v>
@@ -2914,25 +2914,25 @@
         <v>11</v>
       </c>
       <c r="B40" s="3">
-        <v>348</v>
+        <v>532</v>
       </c>
       <c r="C40" s="3">
-        <v>414</v>
+        <v>480</v>
       </c>
       <c r="D40" s="2">
-        <v>103.11</v>
+        <v>30.36</v>
       </c>
       <c r="F40" s="9">
         <v>11</v>
       </c>
       <c r="G40" s="3">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="H40" s="3">
-        <v>202</v>
+        <v>510</v>
       </c>
       <c r="I40" s="2">
-        <v>186.02</v>
+        <v>84.52</v>
       </c>
       <c r="K40" s="9">
         <v>11</v>
@@ -3059,12 +3059,20 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="Z24:AC24"/>
-    <mergeCell ref="Z28:AC28"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="Z3:AC3"/>
-    <mergeCell ref="Z8:AC8"/>
-    <mergeCell ref="Z23:AC23"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F28:I28"/>
     <mergeCell ref="U3:X3"/>
     <mergeCell ref="U4:X4"/>
     <mergeCell ref="U8:X8"/>
@@ -3081,20 +3089,12 @@
     <mergeCell ref="K4:N4"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="P3:S3"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="Z24:AC24"/>
+    <mergeCell ref="Z28:AC28"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="Z23:AC23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>